<commit_message>
Adding the last updates
</commit_message>
<xml_diff>
--- a/OtherDocuments/Notes and to do list.xlsx
+++ b/OtherDocuments/Notes and to do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sossousimpliceadjisse/Documents/myfiles/PaulMoussaReplicationProject/OtherDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE69DEC3-F166-FC40-B1C0-A08E200C789E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FD9129-8B66-C844-B719-B2FD88EEF7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="680" windowWidth="28140" windowHeight="15720" activeTab="5" xr2:uid="{BE3A8758-92C5-B04C-BDD6-5930212A7622}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="445">
   <si>
     <t>Comment</t>
   </si>
@@ -521,9 +521,6 @@
     <t>assessment_bribes.tex</t>
   </si>
   <si>
-    <t xml:space="preserve">Comparing Local and Central on property assignment, bribes, view of government, and view of taxation. </t>
-  </si>
-  <si>
     <t>Descriptive / Testing Local vs Central</t>
   </si>
   <si>
@@ -545,9 +542,6 @@
     <t xml:space="preserve">Causal </t>
   </si>
   <si>
-    <t>783 in MA</t>
-  </si>
-  <si>
     <t>Table 7</t>
   </si>
   <si>
@@ -1278,48 +1272,6 @@
   </si>
   <si>
     <t>Table 9</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Mechanism:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Locals did not do more visits after property registration  or interacted more with cityzens outside of the tax campain  than Central</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Main result:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> CLIs have significantly great compliance and Revenue than Centrals, but did not fully cover the gap with Locals</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1409,20 +1361,119 @@
     <t>776 in MA</t>
   </si>
   <si>
-    <t xml:space="preserve">Re-estimation of Table 4 for Robustness Check controlling for time imbalance </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full saturated estimation of Table 4 with dummies for cross-randomized treatment arms and their interactions with the Local treatment. </t>
-  </si>
-  <si>
     <t>777 in MA</t>
+  </si>
+  <si>
+    <t>Population to which the estimate applies</t>
+  </si>
+  <si>
+    <t>DRC</t>
+  </si>
+  <si>
+    <t>778 in MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results of randomized message in the letters -----&gt; one-fith as much as delagating collectioonf ro city chiefs </t>
+  </si>
+  <si>
+    <t>Any low state capacity environment environment (Country, Region, Province, etc.) with local leadership structure similar to the one of the Kanonga, and where tax collection enforcement is needed.</t>
+  </si>
+  <si>
+    <t>Randomized message contained in the tax letters reminding households they could face fines and be summoned to pay the tax ministry if they did not comply</t>
+  </si>
+  <si>
+    <t>778 In MA</t>
+  </si>
+  <si>
+    <t>Following Miguel and Kremer (2004), we re-estimate the treatment effect while controlling for the number of previously of simultaneously active adjacent neighborhoods with contrasting collector types and the total number of neighborhoods</t>
+  </si>
+  <si>
+    <t>Table4: Competition between collectors (having more adjacebt neighborhoods) is not associated with more taxe compliance ----&gt;&gt;  Re-estimation of Table 4 controlling for externalities of adjacent neighborhoods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 4: Full saturated estimation of Table 4 with dummies for cross-randomized treatment arms and their interactions with the Local treatment. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 4: Further robust estimation of Table 4 by controlling for more covariates. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 4: Re-estimation of Table 4 for Robustness Check controlling for time imbalance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimating if delegating tax collection to chiefs crows our or in contribution to other formal or informal taxes ----&gt; N evidence of such. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiefs are more likely to correctly exempt properties </t>
+  </si>
+  <si>
+    <t>779 in MA</t>
+  </si>
+  <si>
+    <t>If anything, then, Chiefs appear to have respected these rules and procedures of tax campaign more than state collectors.</t>
+  </si>
+  <si>
+    <t>Any low state capacity environment (Country, Region, Province, etc.) with local leadership structure similar to the one of the Kananga, wishing to increase tax revenue and bring long lasting tax compliance culture among it citizens</t>
+  </si>
+  <si>
+    <t>Further examination of Bribes by Chiefs versus Central.</t>
+  </si>
+  <si>
+    <t>Comparing Local and Central on property assignment, bribes, view of government, and view of taxation  -------&gt;&gt;&gt; Chiefs are more likely to correctly exempt properties. They are also more accurate in their assessement of house types. If anything self-reported trust in the government increased by 0.127 standard deviation, but the effect n an aggregate trust index is not different from zero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparing Local to Central, Chiefs do not appear to have made more visits on the extensive or intensive margins </t>
+  </si>
+  <si>
+    <t>782 in MA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Mechanism:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Chiefs did not do more visits after property registration  or interacted more with cityzens outside of the tax campain  than Central -----&gt;&gt; Chief tax collectors do not appear to have achieved higher tax compliance by making more tax appeals.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Mechanism:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> On average, CLI outperformed Central in compliance and revenues. Armed with chiefs information, state collectors achieved 2.4 percentage point higher compliance and 30.9 percentage higher revenue </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1503,6 +1554,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1524,7 +1580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1594,6 +1650,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3036,11 +3095,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B99A516-DB81-4BD9-BF60-5C4B34717121}">
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:J140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3052,10 +3111,12 @@
     <col min="5" max="6" width="57.5" style="15" customWidth="1"/>
     <col min="7" max="7" width="43.6640625" style="15" customWidth="1"/>
     <col min="8" max="8" width="34.5" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="22.83203125" style="15"/>
+    <col min="9" max="9" width="22.83203125" style="15"/>
+    <col min="10" max="10" width="51.33203125" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="22.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>125</v>
       </c>
@@ -3072,39 +3133,45 @@
         <v>129</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>130</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="13" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -3113,7 +3180,7 @@
       <c r="F3" s="12"/>
       <c r="H3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>132</v>
       </c>
@@ -3137,7 +3204,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>138</v>
       </c>
@@ -3161,7 +3228,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>143</v>
       </c>
@@ -3185,7 +3252,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>147</v>
       </c>
@@ -3201,7 +3268,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>147</v>
       </c>
@@ -3217,7 +3284,7 @@
       <c r="E8" s="21"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:9" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>150</v>
       </c>
@@ -3227,9 +3294,9 @@
       <c r="E9" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>151</v>
       </c>
@@ -3243,17 +3310,23 @@
         <v>153</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="15" t="s">
         <v>154</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="23"/>
       <c r="C11" s="14">
@@ -3265,7 +3338,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>156</v>
       </c>
@@ -3279,17 +3352,19 @@
         <v>158</v>
       </c>
       <c r="E12" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15" t="s">
+      <c r="H12" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>147</v>
       </c>
@@ -3300,80 +3375,88 @@
         <v>465</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="B14" s="14" t="s">
         <v>163</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>164</v>
       </c>
       <c r="C14" s="14">
         <v>103</v>
       </c>
       <c r="D14" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>441</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>412</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="15" t="s">
+      <c r="H14" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>169</v>
       </c>
       <c r="C15" s="14">
         <v>137</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>413</v>
+        <v>444</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H15" s="15">
         <v>784</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J15" s="24" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" s="14">
         <v>370</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H16" s="15">
         <v>785</v>
@@ -3390,7 +3473,7 @@
         <v>458</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>147</v>
@@ -3399,23 +3482,23 @@
     </row>
     <row r="18" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C18" s="14">
         <v>554</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F18" s="14"/>
       <c r="I18" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3429,7 +3512,7 @@
         <v>768</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>147</v>
@@ -3438,23 +3521,23 @@
     </row>
     <row r="20" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C20" s="14">
         <v>485</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H20" s="15">
         <v>792</v>
@@ -3462,10 +3545,10 @@
     </row>
     <row r="21" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>147</v>
@@ -3480,10 +3563,10 @@
     </row>
     <row r="22" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>147</v>
@@ -3498,10 +3581,10 @@
     </row>
     <row r="23" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>147</v>
@@ -3516,34 +3599,34 @@
     </row>
     <row r="24" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C24" s="14">
         <v>170</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C25" s="14">
         <v>97</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>147</v>
@@ -3561,7 +3644,7 @@
         <v>213</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>147</v>
@@ -3579,7 +3662,7 @@
         <v>107</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>147</v>
@@ -3597,7 +3680,7 @@
         <v>223</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>147</v>
@@ -3615,7 +3698,7 @@
         <v>117</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>147</v>
@@ -3633,7 +3716,7 @@
         <v>233</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>147</v>
@@ -3642,16 +3725,16 @@
     </row>
     <row r="31" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C31" s="14">
         <v>405</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>147</v>
@@ -3669,7 +3752,7 @@
         <v>472</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>147</v>
@@ -3687,7 +3770,7 @@
         <v>539</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E33" s="14" t="s">
         <v>147</v>
@@ -3696,16 +3779,16 @@
     </row>
     <row r="34" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C34" s="14">
         <v>491</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>147</v>
@@ -3723,7 +3806,7 @@
         <v>642</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>147</v>
@@ -3741,7 +3824,7 @@
         <v>800</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>147</v>
@@ -3750,7 +3833,7 @@
     </row>
     <row r="37" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -3765,16 +3848,16 @@
     </row>
     <row r="38" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C38" s="14">
         <v>452</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>147</v>
@@ -3783,16 +3866,16 @@
     </row>
     <row r="39" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C39" s="14">
         <v>48</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>147</v>
@@ -3801,19 +3884,19 @@
     </row>
     <row r="40" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C40" s="14">
         <v>238</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="F40" s="14"/>
     </row>
@@ -3828,7 +3911,7 @@
         <v>484</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>147</v>
@@ -3837,23 +3920,23 @@
     </row>
     <row r="42" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C42" s="14">
         <v>125</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3867,7 +3950,7 @@
         <v>371</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>147</v>
@@ -3885,7 +3968,7 @@
         <v>619</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>147</v>
@@ -3903,7 +3986,7 @@
         <v>863</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>147</v>
@@ -3912,23 +3995,23 @@
     </row>
     <row r="46" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C46" s="14">
         <v>79</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="F46" s="14"/>
       <c r="H46" s="15" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3942,7 +4025,7 @@
         <v>140</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>147</v>
@@ -3951,23 +4034,23 @@
     </row>
     <row r="48" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C48" s="14">
         <v>322</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>147</v>
+        <v>432</v>
       </c>
       <c r="F48" s="14"/>
     </row>
-    <row r="49" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>147</v>
       </c>
@@ -3978,104 +4061,115 @@
         <v>394</v>
       </c>
       <c r="D49" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B50" s="14" t="s">
         <v>231</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F49" s="14"/>
-    </row>
-    <row r="50" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>233</v>
       </c>
       <c r="C50" s="14">
         <v>573</v>
       </c>
       <c r="D50" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" s="14" t="s">
         <v>234</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F50" s="14"/>
-    </row>
-    <row r="51" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>236</v>
       </c>
       <c r="C51" s="14">
         <v>182</v>
       </c>
       <c r="D51" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="H51" s="15" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F51" s="14"/>
-    </row>
-    <row r="52" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>239</v>
       </c>
       <c r="C52" s="14">
         <v>138</v>
       </c>
       <c r="D52" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B53" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>242</v>
       </c>
       <c r="C53" s="14">
         <v>183</v>
       </c>
       <c r="D53" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B54" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F53" s="14"/>
-    </row>
-    <row r="54" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>245</v>
       </c>
       <c r="C54" s="14">
         <v>178</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F54" s="14"/>
     </row>
-    <row r="55" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
         <v>147</v>
       </c>
@@ -4086,104 +4180,104 @@
         <v>436</v>
       </c>
       <c r="D55" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="B56" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F55" s="14"/>
-    </row>
-    <row r="56" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>249</v>
       </c>
       <c r="C56" s="14">
         <v>31</v>
       </c>
       <c r="D56" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F56" s="14"/>
+    </row>
+    <row r="57" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B57" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F56" s="14"/>
-    </row>
-    <row r="57" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>252</v>
       </c>
       <c r="C57" s="14">
         <v>537</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>147</v>
+        <v>439</v>
       </c>
       <c r="F57" s="14"/>
     </row>
-    <row r="58" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C58" s="14">
         <v>593</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F58" s="14"/>
     </row>
-    <row r="59" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C59" s="14">
         <v>510</v>
       </c>
       <c r="D59" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F59" s="14"/>
+    </row>
+    <row r="60" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B60" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F59" s="14"/>
-    </row>
-    <row r="60" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>259</v>
       </c>
       <c r="C60" s="14">
         <v>372</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E60" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F60" s="14"/>
     </row>
-    <row r="61" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
         <v>147</v>
       </c>
@@ -4194,50 +4288,50 @@
         <v>413</v>
       </c>
       <c r="D61" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F61" s="14"/>
-    </row>
-    <row r="62" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>263</v>
       </c>
       <c r="C62" s="14">
         <v>107</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E62" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F62" s="14"/>
     </row>
-    <row r="63" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C63" s="14">
         <v>732</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E63" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F63" s="14"/>
     </row>
-    <row r="64" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>147</v>
       </c>
@@ -4248,7 +4342,7 @@
         <v>976</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E64" s="14" t="s">
         <v>147</v>
@@ -4257,16 +4351,16 @@
     </row>
     <row r="65" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C65" s="14">
         <v>290</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E65" s="14" t="s">
         <v>147</v>
@@ -4284,7 +4378,7 @@
         <v>290</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E66" s="14" t="s">
         <v>147</v>
@@ -4293,16 +4387,16 @@
     </row>
     <row r="67" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C67" s="14">
         <v>114</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E67" s="14" t="s">
         <v>147</v>
@@ -4311,16 +4405,16 @@
     </row>
     <row r="68" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C68" s="14">
         <v>332</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>147</v>
@@ -4338,7 +4432,7 @@
         <v>410</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>147</v>
@@ -4347,16 +4441,16 @@
     </row>
     <row r="70" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C70" s="14">
         <v>349</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>147</v>
@@ -4374,7 +4468,7 @@
         <v>396</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>147</v>
@@ -4383,16 +4477,16 @@
     </row>
     <row r="72" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C72" s="14">
         <v>113</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>147</v>
@@ -4410,7 +4504,7 @@
         <v>117</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E73" s="14" t="s">
         <v>147</v>
@@ -4428,7 +4522,7 @@
         <v>132</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E74" s="14" t="s">
         <v>147</v>
@@ -4446,7 +4540,7 @@
         <v>136</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E75" s="14" t="s">
         <v>147</v>
@@ -4464,7 +4558,7 @@
         <v>153</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E76" s="14" t="s">
         <v>147</v>
@@ -4482,7 +4576,7 @@
         <v>157</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E77" s="14" t="s">
         <v>147</v>
@@ -4491,16 +4585,16 @@
     </row>
     <row r="78" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C78" s="14">
         <v>234</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E78" s="14" t="s">
         <v>147</v>
@@ -4509,16 +4603,16 @@
     </row>
     <row r="79" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C79" s="14">
         <v>46</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E79" s="14" t="s">
         <v>147</v>
@@ -4527,23 +4621,23 @@
     </row>
     <row r="80" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C80" s="14">
         <v>80</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E80" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F80" s="14"/>
     </row>
-    <row r="81" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
         <v>147</v>
       </c>
@@ -4554,277 +4648,288 @@
         <v>110</v>
       </c>
       <c r="D81" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F81" s="14"/>
+    </row>
+    <row r="82" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="B82" s="14" t="s">
         <v>298</v>
-      </c>
-      <c r="E81" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F81" s="14"/>
-    </row>
-    <row r="82" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="B82" s="14" t="s">
-        <v>300</v>
       </c>
       <c r="C82" s="14">
         <v>132</v>
       </c>
       <c r="D82" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F82" s="14"/>
+    </row>
+    <row r="83" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F83" s="14"/>
+    </row>
+    <row r="84" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="E82" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F82" s="14"/>
-    </row>
-    <row r="83" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E83" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F83" s="14"/>
-    </row>
-    <row r="84" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="14" t="s">
-        <v>303</v>
-      </c>
       <c r="B84" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C84" s="14">
         <v>510</v>
       </c>
       <c r="D84" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F84" s="14"/>
+    </row>
+    <row r="85" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B85" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="E84" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F84" s="14"/>
-    </row>
-    <row r="85" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>306</v>
       </c>
       <c r="C85" s="14">
         <v>64</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F85" s="14"/>
-    </row>
-    <row r="86" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="G85" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H85" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="J85" s="15" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C86" s="14">
         <v>121</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E86" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F86" s="14"/>
     </row>
-    <row r="87" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C87" s="14">
         <v>159</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E87" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F87" s="14"/>
     </row>
-    <row r="88" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C88" s="14">
         <v>197</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E88" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F88" s="14"/>
     </row>
-    <row r="89" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C89" s="14">
         <v>235</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E89" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F89" s="14"/>
     </row>
-    <row r="90" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C90" s="14">
         <v>273</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E90" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F90" s="14"/>
     </row>
-    <row r="91" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C91" s="14">
         <v>315</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E91" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F91" s="14"/>
     </row>
-    <row r="92" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C92" s="14">
         <v>353</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E92" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F92" s="14"/>
     </row>
-    <row r="93" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C93" s="14">
         <v>391</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E93" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F93" s="14"/>
     </row>
-    <row r="94" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C94" s="14">
         <v>429</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E94" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F94" s="14"/>
     </row>
-    <row r="95" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C95" s="14">
         <v>467</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E95" s="14" t="s">
         <v>147</v>
       </c>
       <c r="F95" s="14"/>
     </row>
-    <row r="96" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C96" s="14">
         <v>674</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E96" s="14" t="s">
         <v>147</v>
@@ -4842,7 +4947,7 @@
         <v>890</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E97" s="14" t="s">
         <v>147</v>
@@ -4851,16 +4956,16 @@
     </row>
     <row r="98" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C98" s="14">
         <v>1205</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E98" s="14" t="s">
         <v>147</v>
@@ -4878,7 +4983,7 @@
         <v>1299</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E99" s="14" t="s">
         <v>147</v>
@@ -4887,16 +4992,16 @@
     </row>
     <row r="100" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C100" s="14">
         <v>1004</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E100" s="14" t="s">
         <v>147</v>
@@ -4914,7 +5019,7 @@
         <v>1091</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E101" s="14" t="s">
         <v>147</v>
@@ -4923,16 +5028,16 @@
     </row>
     <row r="102" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C102" s="14">
         <v>438</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E102" s="14" t="s">
         <v>147</v>
@@ -4950,7 +5055,7 @@
         <v>550</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E103" s="14" t="s">
         <v>147</v>
@@ -4968,7 +5073,7 @@
         <v>672</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E104" s="14" t="s">
         <v>147</v>
@@ -4977,16 +5082,16 @@
     </row>
     <row r="105" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C105" s="14">
         <v>138</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E105" s="14" t="s">
         <v>147</v>
@@ -4995,16 +5100,16 @@
     </row>
     <row r="106" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C106" s="14">
         <v>483</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E106" s="14" t="s">
         <v>147</v>
@@ -5013,16 +5118,16 @@
     </row>
     <row r="107" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C107" s="14">
         <v>511</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E107" s="14" t="s">
         <v>147</v>
@@ -5031,16 +5136,16 @@
     </row>
     <row r="108" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C108" s="14">
         <v>452</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E108" s="14" t="s">
         <v>147</v>
@@ -5049,16 +5154,16 @@
     </row>
     <row r="109" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C109" s="14">
         <v>525</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E109" s="14" t="s">
         <v>147</v>
@@ -5076,7 +5181,7 @@
         <v>572</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E110" s="14" t="s">
         <v>147</v>
@@ -5085,16 +5190,16 @@
     </row>
     <row r="111" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C111" s="14">
         <v>435</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E111" s="14" t="s">
         <v>147</v>
@@ -5112,7 +5217,7 @@
         <v>458</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E112" s="14" t="s">
         <v>147</v>
@@ -5130,7 +5235,7 @@
         <v>483</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E113" s="14" t="s">
         <v>147</v>
@@ -5148,7 +5253,7 @@
         <v>506</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E114" s="14" t="s">
         <v>147</v>
@@ -5166,7 +5271,7 @@
         <v>531</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E115" s="14" t="s">
         <v>147</v>
@@ -5184,7 +5289,7 @@
         <v>555</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E116" s="14" t="s">
         <v>147</v>
@@ -5193,16 +5298,16 @@
     </row>
     <row r="117" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="14" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C117" s="14">
         <v>1413</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E117" s="14" t="s">
         <v>147</v>
@@ -5211,16 +5316,16 @@
     </row>
     <row r="118" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C118" s="14">
         <v>299</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E118" s="14" t="s">
         <v>147</v>
@@ -5238,7 +5343,7 @@
         <v>358</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E119" s="14" t="s">
         <v>147</v>
@@ -5256,7 +5361,7 @@
         <v>420</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E120" s="14" t="s">
         <v>147</v>
@@ -5265,16 +5370,16 @@
     </row>
     <row r="121" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C121" s="14">
         <v>311</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E121" s="14" t="s">
         <v>147</v>
@@ -5292,7 +5397,7 @@
         <v>343</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E122" s="14" t="s">
         <v>147</v>
@@ -5301,16 +5406,16 @@
     </row>
     <row r="123" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C123" s="14">
         <v>113</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E123" s="14" t="s">
         <v>147</v>
@@ -5328,7 +5433,7 @@
         <v>117</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E124" s="14" t="s">
         <v>147</v>
@@ -5337,10 +5442,10 @@
     </row>
     <row r="125" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C125" s="14" t="s">
         <v>147</v>
@@ -5355,10 +5460,10 @@
     </row>
     <row r="126" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C126" s="14" t="s">
         <v>147</v>
@@ -5373,16 +5478,16 @@
     </row>
     <row r="127" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C127" s="14">
         <v>49</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E127" s="14" t="s">
         <v>147</v>
@@ -5394,16 +5499,16 @@
     </row>
     <row r="128" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="14" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C128" s="14">
         <v>163</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E128" s="14" t="s">
         <v>147</v>
@@ -5415,16 +5520,16 @@
     </row>
     <row r="129" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C129" s="14">
         <v>108</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E129" s="14" t="s">
         <v>147</v>
@@ -5436,16 +5541,16 @@
     </row>
     <row r="130" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C130" s="14">
         <v>305</v>
       </c>
       <c r="D130" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E130" s="14" t="s">
         <v>147</v>
@@ -5457,16 +5562,16 @@
     </row>
     <row r="131" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C131" s="14">
         <v>240</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E131" s="14" t="s">
         <v>147</v>
@@ -5478,16 +5583,16 @@
     </row>
     <row r="132" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C132" s="14">
         <v>623</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E132" s="14" t="s">
         <v>147</v>
@@ -5499,16 +5604,16 @@
     </row>
     <row r="133" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C133" s="14">
         <v>486</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E133" s="14" t="s">
         <v>147</v>
@@ -5520,16 +5625,16 @@
     </row>
     <row r="134" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C134" s="14">
         <v>533</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E134" s="14" t="s">
         <v>147</v>
@@ -5541,16 +5646,16 @@
     </row>
     <row r="135" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C135" s="14">
         <v>191</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E135" s="14" t="s">
         <v>147</v>
@@ -5562,16 +5667,16 @@
     </row>
     <row r="136" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C136" s="14">
         <v>25</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E136" s="14" t="s">
         <v>147</v>
@@ -5583,16 +5688,16 @@
     </row>
     <row r="137" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C137" s="16">
         <v>96</v>
       </c>
       <c r="D137" s="16" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E137" s="14" t="s">
         <v>147</v>
@@ -5604,13 +5709,13 @@
     </row>
     <row r="138" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="16" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C138" s="16">
         <v>64</v>
       </c>
       <c r="D138" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G138" s="15" t="s">
         <v>136</v>
@@ -5618,16 +5723,16 @@
     </row>
     <row r="139" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C139" s="14">
         <v>71</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E139" s="14" t="s">
         <v>147</v>
@@ -5639,16 +5744,16 @@
     </row>
     <row r="140" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C140" s="14">
         <v>168</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E140" s="14" t="s">
         <v>147</v>
@@ -5683,22 +5788,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the last changes
</commit_message>
<xml_diff>
--- a/OtherDocuments/Notes and to do list.xlsx
+++ b/OtherDocuments/Notes and to do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sossousimpliceadjisse/Documents/myfiles/PaulMoussaReplicationProject/OtherDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FD9129-8B66-C844-B719-B2FD88EEF7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5B3E6C-E549-6042-BAE9-45FD814607C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="680" windowWidth="28140" windowHeight="15720" activeTab="5" xr2:uid="{BE3A8758-92C5-B04C-BDD6-5930212A7622}"/>
   </bookViews>
@@ -3097,9 +3097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B99A516-DB81-4BD9-BF60-5C4B34717121}">
   <dimension ref="A1:J140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3167,7 +3167,7 @@
       <c r="H2" s="24" t="s">
         <v>414</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="24" t="s">
         <v>438</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Table8R2, replication using ordered probit
</commit_message>
<xml_diff>
--- a/OtherDocuments/Notes and to do list.xlsx
+++ b/OtherDocuments/Notes and to do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sossousimpliceadjisse/Documents/myfiles/PaulMoussaReplicationProject/OtherDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5B3E6C-E549-6042-BAE9-45FD814607C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1921B1CB-DB11-774D-A41F-41AB0DD2B0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="680" windowWidth="28140" windowHeight="15720" activeTab="5" xr2:uid="{BE3A8758-92C5-B04C-BDD6-5930212A7622}"/>
   </bookViews>
@@ -3098,8 +3098,8 @@
   <dimension ref="A1:J140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding the Replication of the Table 8LCC and other materials
</commit_message>
<xml_diff>
--- a/OtherDocuments/Notes and to do list.xlsx
+++ b/OtherDocuments/Notes and to do list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sossousimpliceadjisse/Documents/myfiles/PaulMoussaReplicationProject/OtherDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5115837F-7681-A24D-877D-539BB25E94A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB56294-6F82-394A-B56E-0407C431A616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="680" windowWidth="28140" windowHeight="15720" activeTab="5" xr2:uid="{BE3A8758-92C5-B04C-BDD6-5930212A7622}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="453">
   <si>
     <t>Comment</t>
   </si>
@@ -1470,6 +1470,27 @@
       </rPr>
       <t>: Average treatment effect of the "Local treatment" tax collection derives heavily from higher compliance among low-value properties.</t>
     </r>
+  </si>
+  <si>
+    <t>Claim 1</t>
+  </si>
+  <si>
+    <t>Claim 2</t>
+  </si>
+  <si>
+    <t>Claim 3</t>
+  </si>
+  <si>
+    <t>Claim 4</t>
+  </si>
+  <si>
+    <t>Claim 5</t>
+  </si>
+  <si>
+    <t>Claim 6</t>
+  </si>
+  <si>
+    <t>No Claim</t>
   </si>
 </sst>
 </file>
@@ -1685,7 +1706,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1973,7 +1994,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3107,11 +3128,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B99A516-DB81-4BD9-BF60-5C4B34717121}">
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3119,16 +3140,16 @@
     <col min="1" max="1" width="18.6640625" style="15" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" style="15" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="53" style="15" customWidth="1"/>
-    <col min="5" max="6" width="57.5" style="15" customWidth="1"/>
-    <col min="7" max="7" width="43.6640625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="34.5" style="15" customWidth="1"/>
-    <col min="9" max="9" width="22.83203125" style="15"/>
-    <col min="10" max="10" width="51.33203125" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="22.83203125" style="15"/>
+    <col min="4" max="5" width="53" style="15" customWidth="1"/>
+    <col min="6" max="7" width="57.5" style="15" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="34.5" style="15" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="15"/>
+    <col min="11" max="11" width="51.33203125" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="22.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>125</v>
       </c>
@@ -3142,57 +3163,62 @@
         <v>128</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>415</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>410</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>416</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>412</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="12"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>132</v>
       </c>
@@ -3205,18 +3231,19 @@
       <c r="D4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>138</v>
       </c>
@@ -3229,18 +3256,19 @@
       <c r="D5" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>143</v>
       </c>
@@ -3253,18 +3281,19 @@
       <c r="D6" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14"/>
+      <c r="H6" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="H6" s="15">
+      <c r="I6" s="15">
         <v>777</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>147</v>
       </c>
@@ -3277,10 +3306,11 @@
       <c r="D7" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E7" s="14"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>147</v>
       </c>
@@ -3293,22 +3323,24 @@
       <c r="D8" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="14"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>150</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>151</v>
       </c>
@@ -3321,24 +3353,27 @@
       <c r="D10" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>439</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="18"/>
+      <c r="H10" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>417</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="15" t="s">
         <v>420</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="K10" s="22" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
       <c r="B11" s="26"/>
       <c r="C11" s="14">
@@ -3347,10 +3382,11 @@
       <c r="D11" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="14"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>156</v>
       </c>
@@ -3363,23 +3399,26 @@
       <c r="D12" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>441</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="G12" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="H12" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="I12" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="K12" s="22" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>147</v>
       </c>
@@ -3392,12 +3431,13 @@
       <c r="D13" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>162</v>
       </c>
@@ -3410,23 +3450,26 @@
       <c r="D14" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>442</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="G14" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="H14" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="I14" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="K14" s="22" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>166</v>
       </c>
@@ -3439,21 +3482,24 @@
       <c r="D15" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="19"/>
+      <c r="H15" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="H15" s="15">
+      <c r="I15" s="15">
         <v>784</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="K15" s="22" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>169</v>
       </c>
@@ -3466,21 +3512,24 @@
       <c r="D16" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>444</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="19"/>
+      <c r="H16" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="H16" s="15">
+      <c r="I16" s="15">
         <v>785</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="K16" s="22" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>147</v>
       </c>
@@ -3493,12 +3542,13 @@
       <c r="D17" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>173</v>
       </c>
@@ -3511,15 +3561,16 @@
       <c r="D18" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="I18" s="15" t="s">
+      <c r="E18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="J18" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>147</v>
       </c>
@@ -3532,12 +3583,13 @@
       <c r="D19" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>178</v>
       </c>
@@ -3550,21 +3602,24 @@
       <c r="D20" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="14" t="s">
+        <v>451</v>
+      </c>
+      <c r="F20" s="19" t="s">
         <v>445</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="19"/>
+      <c r="H20" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="H20" s="15">
+      <c r="I20" s="15">
         <v>792</v>
       </c>
-      <c r="J20" s="22" t="s">
+      <c r="K20" s="22" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>181</v>
       </c>
@@ -3577,12 +3632,13 @@
       <c r="D21" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>183</v>
       </c>
@@ -3595,12 +3651,13 @@
       <c r="D22" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>184</v>
       </c>
@@ -3613,13 +3670,14 @@
       <c r="D23" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>185</v>
       </c>
@@ -3632,12 +3690,13 @@
       <c r="D24" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="14"/>
+      <c r="F24" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>189</v>
       </c>
@@ -3650,12 +3709,13 @@
       <c r="D25" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F25" s="14"/>
-    </row>
-    <row r="26" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="14"/>
+      <c r="F25" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>147</v>
       </c>
@@ -3668,12 +3728,13 @@
       <c r="D26" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" s="14"/>
-    </row>
-    <row r="27" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>147</v>
       </c>
@@ -3686,12 +3747,13 @@
       <c r="D27" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="E27" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="14"/>
+      <c r="F27" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>147</v>
       </c>
@@ -3704,12 +3766,13 @@
       <c r="D28" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="E28" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="14"/>
+      <c r="F28" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>147</v>
       </c>
@@ -3722,12 +3785,13 @@
       <c r="D29" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" s="14"/>
+    </row>
+    <row r="30" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>147</v>
       </c>
@@ -3740,12 +3804,13 @@
       <c r="D30" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E30" s="14"/>
+      <c r="F30" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>197</v>
       </c>
@@ -3758,12 +3823,13 @@
       <c r="D31" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E31" s="14"/>
+      <c r="F31" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>147</v>
       </c>
@@ -3776,12 +3842,13 @@
       <c r="D32" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="E32" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E32" s="14"/>
+      <c r="F32" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>147</v>
       </c>
@@ -3794,12 +3861,13 @@
       <c r="D33" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="14"/>
+      <c r="F33" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>202</v>
       </c>
@@ -3812,12 +3880,13 @@
       <c r="D34" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="E34" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F34" s="14"/>
-    </row>
-    <row r="35" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E34" s="14"/>
+      <c r="F34" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>147</v>
       </c>
@@ -3830,12 +3899,13 @@
       <c r="D35" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>147</v>
       </c>
@@ -3848,27 +3918,29 @@
       <c r="D36" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="E36" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E36" s="14"/>
+      <c r="F36" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="24" t="s">
         <v>206</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
-      <c r="E37" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="15" t="s">
+      <c r="E37" s="14"/>
+      <c r="F37" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>207</v>
       </c>
@@ -3881,12 +3953,13 @@
       <c r="D38" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="E38" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="14"/>
+      <c r="F38" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>210</v>
       </c>
@@ -3899,12 +3972,13 @@
       <c r="D39" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="E39" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E39" s="14"/>
+      <c r="F39" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>213</v>
       </c>
@@ -3917,12 +3991,13 @@
       <c r="D40" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="14"/>
+      <c r="F40" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>147</v>
       </c>
@@ -3935,12 +4010,13 @@
       <c r="D41" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="E41" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F41" s="14"/>
-    </row>
-    <row r="42" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E41" s="14"/>
+      <c r="F41" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>217</v>
       </c>
@@ -3953,15 +4029,16 @@
       <c r="D42" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="E42" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F42" s="14"/>
-      <c r="G42" s="15" t="s">
+      <c r="E42" s="14"/>
+      <c r="F42" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="15" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>147</v>
       </c>
@@ -3974,12 +4051,13 @@
       <c r="D43" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="E43" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F43" s="14"/>
-    </row>
-    <row r="44" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E43" s="14"/>
+      <c r="F43" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>147</v>
       </c>
@@ -3992,12 +4070,13 @@
       <c r="D44" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="E44" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E44" s="14"/>
+      <c r="F44" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>147</v>
       </c>
@@ -4010,12 +4089,13 @@
       <c r="D45" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E45" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F45" s="14"/>
-    </row>
-    <row r="46" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E45" s="14"/>
+      <c r="F45" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>222</v>
       </c>
@@ -4028,15 +4108,16 @@
       <c r="D46" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="14"/>
+      <c r="F46" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="F46" s="14"/>
-      <c r="H46" s="15" t="s">
+      <c r="G46" s="14"/>
+      <c r="I46" s="15" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>147</v>
       </c>
@@ -4049,12 +4130,13 @@
       <c r="D47" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E47" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F47" s="14"/>
-    </row>
-    <row r="48" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E47" s="14"/>
+      <c r="F47" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" s="14"/>
+    </row>
+    <row r="48" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>226</v>
       </c>
@@ -4067,12 +4149,13 @@
       <c r="D48" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="14"/>
+      <c r="F48" s="14" t="s">
         <v>429</v>
       </c>
-      <c r="F48" s="14"/>
-    </row>
-    <row r="49" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>147</v>
       </c>
@@ -4085,12 +4168,13 @@
       <c r="D49" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="E49" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F49" s="14"/>
-    </row>
-    <row r="50" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E49" s="14"/>
+      <c r="F49" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>230</v>
       </c>
@@ -4103,12 +4187,13 @@
       <c r="D50" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="E50" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F50" s="14"/>
-    </row>
-    <row r="51" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E50" s="14"/>
+      <c r="F50" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>233</v>
       </c>
@@ -4121,15 +4206,16 @@
       <c r="D51" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="14"/>
+      <c r="F51" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="F51" s="14"/>
-      <c r="H51" s="15" t="s">
+      <c r="G51" s="14"/>
+      <c r="I51" s="15" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>236</v>
       </c>
@@ -4142,20 +4228,21 @@
       <c r="D52" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="14"/>
+      <c r="F52" s="14" t="s">
         <v>427</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="G52" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="H52" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="H52" s="15" t="s">
+      <c r="I52" s="15" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>239</v>
       </c>
@@ -4168,12 +4255,13 @@
       <c r="D53" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="14"/>
+      <c r="F53" s="14" t="s">
         <v>431</v>
       </c>
-      <c r="F53" s="14"/>
-    </row>
-    <row r="54" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G53" s="14"/>
+    </row>
+    <row r="54" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>242</v>
       </c>
@@ -4186,12 +4274,13 @@
       <c r="D54" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="E54" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F54" s="14"/>
-    </row>
-    <row r="55" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E54" s="14"/>
+      <c r="F54" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G54" s="14"/>
+    </row>
+    <row r="55" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
         <v>147</v>
       </c>
@@ -4204,12 +4293,13 @@
       <c r="D55" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="E55" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F55" s="14"/>
-    </row>
-    <row r="56" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E55" s="14"/>
+      <c r="F55" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G55" s="14"/>
+    </row>
+    <row r="56" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
         <v>246</v>
       </c>
@@ -4222,12 +4312,13 @@
       <c r="D56" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="E56" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F56" s="14"/>
-    </row>
-    <row r="57" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E56" s="14"/>
+      <c r="F56" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" s="14"/>
+    </row>
+    <row r="57" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>249</v>
       </c>
@@ -4240,12 +4331,13 @@
       <c r="D57" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="E57" s="14"/>
+      <c r="F57" s="14" t="s">
         <v>436</v>
       </c>
-      <c r="F57" s="14"/>
-    </row>
-    <row r="58" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G57" s="14"/>
+    </row>
+    <row r="58" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>252</v>
       </c>
@@ -4258,12 +4350,13 @@
       <c r="D58" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="E58" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F58" s="14"/>
-    </row>
-    <row r="59" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E58" s="14"/>
+      <c r="F58" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G58" s="14"/>
+    </row>
+    <row r="59" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
         <v>254</v>
       </c>
@@ -4276,12 +4369,13 @@
       <c r="D59" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E59" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F59" s="14"/>
-    </row>
-    <row r="60" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E59" s="14"/>
+      <c r="F59" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G59" s="14"/>
+    </row>
+    <row r="60" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
         <v>256</v>
       </c>
@@ -4294,12 +4388,13 @@
       <c r="D60" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="E60" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F60" s="14"/>
-    </row>
-    <row r="61" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E60" s="14"/>
+      <c r="F60" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G60" s="14"/>
+    </row>
+    <row r="61" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
         <v>147</v>
       </c>
@@ -4312,12 +4407,13 @@
       <c r="D61" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E61" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F61" s="14"/>
-    </row>
-    <row r="62" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E61" s="14"/>
+      <c r="F61" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G61" s="14"/>
+    </row>
+    <row r="62" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>260</v>
       </c>
@@ -4330,12 +4426,13 @@
       <c r="D62" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="E62" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F62" s="14"/>
-    </row>
-    <row r="63" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E62" s="14"/>
+      <c r="F62" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G62" s="14"/>
+    </row>
+    <row r="63" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
         <v>263</v>
       </c>
@@ -4348,12 +4445,13 @@
       <c r="D63" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="E63" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F63" s="14"/>
-    </row>
-    <row r="64" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E63" s="14"/>
+      <c r="F63" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G63" s="14"/>
+    </row>
+    <row r="64" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>147</v>
       </c>
@@ -4366,12 +4464,13 @@
       <c r="D64" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="E64" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F64" s="14"/>
-    </row>
-    <row r="65" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E64" s="14"/>
+      <c r="F64" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G64" s="14"/>
+    </row>
+    <row r="65" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>266</v>
       </c>
@@ -4384,12 +4483,13 @@
       <c r="D65" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="E65" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F65" s="14"/>
-    </row>
-    <row r="66" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E65" s="14"/>
+      <c r="F65" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G65" s="14"/>
+    </row>
+    <row r="66" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
         <v>147</v>
       </c>
@@ -4402,12 +4502,13 @@
       <c r="D66" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="E66" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F66" s="14"/>
-    </row>
-    <row r="67" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E66" s="14"/>
+      <c r="F66" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G66" s="14"/>
+    </row>
+    <row r="67" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
         <v>270</v>
       </c>
@@ -4420,12 +4521,13 @@
       <c r="D67" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="E67" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F67" s="14"/>
-    </row>
-    <row r="68" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E67" s="14"/>
+      <c r="F67" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G67" s="14"/>
+    </row>
+    <row r="68" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
         <v>273</v>
       </c>
@@ -4438,12 +4540,13 @@
       <c r="D68" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="E68" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F68" s="14"/>
-    </row>
-    <row r="69" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E68" s="14"/>
+      <c r="F68" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G68" s="14"/>
+    </row>
+    <row r="69" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="14" t="s">
         <v>147</v>
       </c>
@@ -4456,12 +4559,13 @@
       <c r="D69" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="E69" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F69" s="14"/>
-    </row>
-    <row r="70" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E69" s="14"/>
+      <c r="F69" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G69" s="14"/>
+    </row>
+    <row r="70" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
         <v>277</v>
       </c>
@@ -4474,12 +4578,13 @@
       <c r="D70" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="E70" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F70" s="14"/>
-    </row>
-    <row r="71" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E70" s="14"/>
+      <c r="F70" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G70" s="14"/>
+    </row>
+    <row r="71" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
         <v>147</v>
       </c>
@@ -4492,12 +4597,13 @@
       <c r="D71" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E71" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F71" s="14"/>
-    </row>
-    <row r="72" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E71" s="14"/>
+      <c r="F71" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G71" s="14"/>
+    </row>
+    <row r="72" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="14" t="s">
         <v>281</v>
       </c>
@@ -4510,12 +4616,13 @@
       <c r="D72" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="E72" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F72" s="14"/>
-    </row>
-    <row r="73" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E72" s="14"/>
+      <c r="F72" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G72" s="14"/>
+    </row>
+    <row r="73" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
         <v>147</v>
       </c>
@@ -4528,12 +4635,13 @@
       <c r="D73" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="E73" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F73" s="14"/>
-    </row>
-    <row r="74" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E73" s="14"/>
+      <c r="F73" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G73" s="14"/>
+    </row>
+    <row r="74" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>147</v>
       </c>
@@ -4546,12 +4654,13 @@
       <c r="D74" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="E74" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F74" s="14"/>
-    </row>
-    <row r="75" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E74" s="14"/>
+      <c r="F74" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G74" s="14"/>
+    </row>
+    <row r="75" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
         <v>147</v>
       </c>
@@ -4564,12 +4673,13 @@
       <c r="D75" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="E75" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F75" s="14"/>
-    </row>
-    <row r="76" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E75" s="14"/>
+      <c r="F75" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G75" s="14"/>
+    </row>
+    <row r="76" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
         <v>147</v>
       </c>
@@ -4582,12 +4692,13 @@
       <c r="D76" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="E76" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F76" s="14"/>
-    </row>
-    <row r="77" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E76" s="14"/>
+      <c r="F76" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G76" s="14"/>
+    </row>
+    <row r="77" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
         <v>147</v>
       </c>
@@ -4600,12 +4711,13 @@
       <c r="D77" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="E77" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F77" s="14"/>
-    </row>
-    <row r="78" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E77" s="14"/>
+      <c r="F77" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G77" s="14"/>
+    </row>
+    <row r="78" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
         <v>289</v>
       </c>
@@ -4618,12 +4730,13 @@
       <c r="D78" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="E78" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F78" s="14"/>
-    </row>
-    <row r="79" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E78" s="14"/>
+      <c r="F78" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G78" s="14"/>
+    </row>
+    <row r="79" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
         <v>291</v>
       </c>
@@ -4636,12 +4749,13 @@
       <c r="D79" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="E79" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F79" s="14"/>
-    </row>
-    <row r="80" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E79" s="14"/>
+      <c r="F79" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G79" s="14"/>
+    </row>
+    <row r="80" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
         <v>294</v>
       </c>
@@ -4654,12 +4768,13 @@
       <c r="D80" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="E80" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F80" s="14"/>
-    </row>
-    <row r="81" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E80" s="14"/>
+      <c r="F80" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G80" s="14"/>
+    </row>
+    <row r="81" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
         <v>147</v>
       </c>
@@ -4672,12 +4787,13 @@
       <c r="D81" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="E81" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F81" s="14"/>
-    </row>
-    <row r="82" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E81" s="14"/>
+      <c r="F81" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G81" s="14"/>
+    </row>
+    <row r="82" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>297</v>
       </c>
@@ -4690,12 +4806,13 @@
       <c r="D82" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="E82" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F82" s="14"/>
-    </row>
-    <row r="83" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E82" s="14"/>
+      <c r="F82" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G82" s="14"/>
+    </row>
+    <row r="83" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
         <v>300</v>
       </c>
@@ -4708,12 +4825,13 @@
       <c r="D83" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E83" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F83" s="14"/>
-    </row>
-    <row r="84" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E83" s="14"/>
+      <c r="F83" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G83" s="14"/>
+    </row>
+    <row r="84" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
         <v>301</v>
       </c>
@@ -4726,12 +4844,13 @@
       <c r="D84" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="E84" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F84" s="14"/>
-    </row>
-    <row r="85" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E84" s="14"/>
+      <c r="F84" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G84" s="14"/>
+    </row>
+    <row r="85" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
         <v>303</v>
       </c>
@@ -4744,23 +4863,24 @@
       <c r="D85" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="E85" s="14" t="s">
+      <c r="E85" s="14"/>
+      <c r="F85" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="F85" s="14" t="s">
+      <c r="G85" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="G85" s="15" t="s">
+      <c r="H85" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="H85" s="15" t="s">
+      <c r="I85" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="J85" s="15" t="s">
+      <c r="K85" s="15" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
         <v>306</v>
       </c>
@@ -4773,12 +4893,13 @@
       <c r="D86" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="E86" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F86" s="14"/>
-    </row>
-    <row r="87" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E86" s="14"/>
+      <c r="F86" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G86" s="14"/>
+    </row>
+    <row r="87" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
         <v>147</v>
       </c>
@@ -4791,12 +4912,13 @@
       <c r="D87" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="E87" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F87" s="14"/>
-    </row>
-    <row r="88" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E87" s="14"/>
+      <c r="F87" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G87" s="14"/>
+    </row>
+    <row r="88" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
         <v>147</v>
       </c>
@@ -4809,12 +4931,13 @@
       <c r="D88" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="E88" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F88" s="14"/>
-    </row>
-    <row r="89" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E88" s="14"/>
+      <c r="F88" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G88" s="14"/>
+    </row>
+    <row r="89" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="14" t="s">
         <v>147</v>
       </c>
@@ -4827,12 +4950,13 @@
       <c r="D89" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="E89" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F89" s="14"/>
-    </row>
-    <row r="90" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E89" s="14"/>
+      <c r="F89" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G89" s="14"/>
+    </row>
+    <row r="90" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
         <v>147</v>
       </c>
@@ -4845,12 +4969,13 @@
       <c r="D90" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="E90" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F90" s="14"/>
-    </row>
-    <row r="91" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E90" s="14"/>
+      <c r="F90" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G90" s="14"/>
+    </row>
+    <row r="91" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
         <v>312</v>
       </c>
@@ -4863,12 +4988,13 @@
       <c r="D91" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="E91" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F91" s="14"/>
-    </row>
-    <row r="92" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E91" s="14"/>
+      <c r="F91" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G91" s="14"/>
+    </row>
+    <row r="92" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
         <v>147</v>
       </c>
@@ -4881,12 +5007,13 @@
       <c r="D92" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="E92" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F92" s="14"/>
-    </row>
-    <row r="93" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E92" s="14"/>
+      <c r="F92" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G92" s="14"/>
+    </row>
+    <row r="93" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
         <v>147</v>
       </c>
@@ -4899,12 +5026,13 @@
       <c r="D93" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="E93" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F93" s="14"/>
-    </row>
-    <row r="94" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E93" s="14"/>
+      <c r="F93" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G93" s="14"/>
+    </row>
+    <row r="94" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
         <v>147</v>
       </c>
@@ -4917,12 +5045,13 @@
       <c r="D94" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="E94" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F94" s="14"/>
-    </row>
-    <row r="95" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E94" s="14"/>
+      <c r="F94" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G94" s="14"/>
+    </row>
+    <row r="95" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
         <v>147</v>
       </c>
@@ -4935,12 +5064,13 @@
       <c r="D95" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="E95" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F95" s="14"/>
-    </row>
-    <row r="96" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E95" s="14"/>
+      <c r="F95" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G95" s="14"/>
+    </row>
+    <row r="96" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
         <v>318</v>
       </c>
@@ -4953,12 +5083,13 @@
       <c r="D96" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="E96" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F96" s="14"/>
-    </row>
-    <row r="97" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E96" s="14"/>
+      <c r="F96" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G96" s="14"/>
+    </row>
+    <row r="97" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="14" t="s">
         <v>147</v>
       </c>
@@ -4971,12 +5102,13 @@
       <c r="D97" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="E97" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F97" s="14"/>
-    </row>
-    <row r="98" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E97" s="14"/>
+      <c r="F97" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G97" s="14"/>
+    </row>
+    <row r="98" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
         <v>321</v>
       </c>
@@ -4989,12 +5121,13 @@
       <c r="D98" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="E98" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F98" s="14"/>
-    </row>
-    <row r="99" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E98" s="14"/>
+      <c r="F98" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G98" s="14"/>
+    </row>
+    <row r="99" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="14" t="s">
         <v>147</v>
       </c>
@@ -5007,12 +5140,13 @@
       <c r="D99" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="E99" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F99" s="14"/>
-    </row>
-    <row r="100" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E99" s="14"/>
+      <c r="F99" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G99" s="14"/>
+    </row>
+    <row r="100" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="14" t="s">
         <v>324</v>
       </c>
@@ -5025,12 +5159,13 @@
       <c r="D100" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="E100" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F100" s="14"/>
-    </row>
-    <row r="101" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E100" s="14"/>
+      <c r="F100" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G100" s="14"/>
+    </row>
+    <row r="101" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="14" t="s">
         <v>147</v>
       </c>
@@ -5043,12 +5178,13 @@
       <c r="D101" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="E101" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F101" s="14"/>
-    </row>
-    <row r="102" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E101" s="14"/>
+      <c r="F101" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G101" s="14"/>
+    </row>
+    <row r="102" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="14" t="s">
         <v>327</v>
       </c>
@@ -5061,12 +5197,13 @@
       <c r="D102" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="E102" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F102" s="14"/>
-    </row>
-    <row r="103" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E102" s="14"/>
+      <c r="F102" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G102" s="14"/>
+    </row>
+    <row r="103" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="14" t="s">
         <v>147</v>
       </c>
@@ -5079,12 +5216,13 @@
       <c r="D103" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="E103" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F103" s="14"/>
-    </row>
-    <row r="104" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E103" s="14"/>
+      <c r="F103" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G103" s="14"/>
+    </row>
+    <row r="104" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="14" t="s">
         <v>147</v>
       </c>
@@ -5097,12 +5235,13 @@
       <c r="D104" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="E104" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F104" s="14"/>
-    </row>
-    <row r="105" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E104" s="14"/>
+      <c r="F104" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G104" s="14"/>
+    </row>
+    <row r="105" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="14" t="s">
         <v>332</v>
       </c>
@@ -5115,12 +5254,13 @@
       <c r="D105" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="E105" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F105" s="14"/>
-    </row>
-    <row r="106" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E105" s="14"/>
+      <c r="F105" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G105" s="14"/>
+    </row>
+    <row r="106" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="14" t="s">
         <v>335</v>
       </c>
@@ -5133,12 +5273,13 @@
       <c r="D106" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="E106" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F106" s="14"/>
-    </row>
-    <row r="107" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E106" s="14"/>
+      <c r="F106" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G106" s="14"/>
+    </row>
+    <row r="107" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
         <v>338</v>
       </c>
@@ -5151,12 +5292,13 @@
       <c r="D107" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="E107" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F107" s="14"/>
-    </row>
-    <row r="108" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E107" s="14"/>
+      <c r="F107" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G107" s="14"/>
+    </row>
+    <row r="108" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
         <v>341</v>
       </c>
@@ -5169,12 +5311,13 @@
       <c r="D108" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="E108" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F108" s="14"/>
-    </row>
-    <row r="109" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E108" s="14"/>
+      <c r="F108" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G108" s="14"/>
+    </row>
+    <row r="109" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="14" t="s">
         <v>344</v>
       </c>
@@ -5187,12 +5330,13 @@
       <c r="D109" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="E109" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F109" s="14"/>
-    </row>
-    <row r="110" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E109" s="14"/>
+      <c r="F109" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G109" s="14"/>
+    </row>
+    <row r="110" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="14" t="s">
         <v>147</v>
       </c>
@@ -5205,12 +5349,13 @@
       <c r="D110" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="E110" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F110" s="14"/>
-    </row>
-    <row r="111" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E110" s="14"/>
+      <c r="F110" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G110" s="14"/>
+    </row>
+    <row r="111" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="14" t="s">
         <v>347</v>
       </c>
@@ -5223,12 +5368,13 @@
       <c r="D111" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="E111" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F111" s="14"/>
-    </row>
-    <row r="112" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E111" s="14"/>
+      <c r="F111" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G111" s="14"/>
+    </row>
+    <row r="112" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="14" t="s">
         <v>147</v>
       </c>
@@ -5241,12 +5387,13 @@
       <c r="D112" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="E112" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F112" s="14"/>
-    </row>
-    <row r="113" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E112" s="14"/>
+      <c r="F112" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G112" s="14"/>
+    </row>
+    <row r="113" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="14" t="s">
         <v>147</v>
       </c>
@@ -5259,12 +5406,13 @@
       <c r="D113" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="E113" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F113" s="14"/>
-    </row>
-    <row r="114" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E113" s="14"/>
+      <c r="F113" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G113" s="14"/>
+    </row>
+    <row r="114" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="14" t="s">
         <v>147</v>
       </c>
@@ -5277,12 +5425,13 @@
       <c r="D114" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="E114" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F114" s="14"/>
-    </row>
-    <row r="115" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E114" s="14"/>
+      <c r="F114" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G114" s="14"/>
+    </row>
+    <row r="115" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="14" t="s">
         <v>147</v>
       </c>
@@ -5295,12 +5444,13 @@
       <c r="D115" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="E115" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F115" s="14"/>
-    </row>
-    <row r="116" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E115" s="14"/>
+      <c r="F115" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G115" s="14"/>
+    </row>
+    <row r="116" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="14" t="s">
         <v>147</v>
       </c>
@@ -5313,12 +5463,13 @@
       <c r="D116" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="E116" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F116" s="14"/>
-    </row>
-    <row r="117" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E116" s="14"/>
+      <c r="F116" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G116" s="14"/>
+    </row>
+    <row r="117" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="14" t="s">
         <v>355</v>
       </c>
@@ -5331,12 +5482,13 @@
       <c r="D117" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="E117" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F117" s="14"/>
-    </row>
-    <row r="118" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E117" s="14"/>
+      <c r="F117" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G117" s="14"/>
+    </row>
+    <row r="118" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="14" t="s">
         <v>357</v>
       </c>
@@ -5349,12 +5501,13 @@
       <c r="D118" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="E118" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F118" s="14"/>
-    </row>
-    <row r="119" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E118" s="14"/>
+      <c r="F118" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G118" s="14"/>
+    </row>
+    <row r="119" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="14" t="s">
         <v>147</v>
       </c>
@@ -5367,12 +5520,13 @@
       <c r="D119" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="E119" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F119" s="14"/>
-    </row>
-    <row r="120" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E119" s="14"/>
+      <c r="F119" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G119" s="14"/>
+    </row>
+    <row r="120" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="14" t="s">
         <v>147</v>
       </c>
@@ -5385,12 +5539,13 @@
       <c r="D120" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="E120" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F120" s="14"/>
-    </row>
-    <row r="121" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E120" s="14"/>
+      <c r="F120" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G120" s="14"/>
+    </row>
+    <row r="121" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="14" t="s">
         <v>362</v>
       </c>
@@ -5403,12 +5558,13 @@
       <c r="D121" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="E121" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F121" s="14"/>
-    </row>
-    <row r="122" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E121" s="14"/>
+      <c r="F121" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G121" s="14"/>
+    </row>
+    <row r="122" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="14" t="s">
         <v>147</v>
       </c>
@@ -5421,12 +5577,13 @@
       <c r="D122" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="E122" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F122" s="14"/>
-    </row>
-    <row r="123" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E122" s="14"/>
+      <c r="F122" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G122" s="14"/>
+    </row>
+    <row r="123" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="14" t="s">
         <v>366</v>
       </c>
@@ -5439,12 +5596,13 @@
       <c r="D123" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="E123" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F123" s="14"/>
-    </row>
-    <row r="124" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E123" s="14"/>
+      <c r="F123" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G123" s="14"/>
+    </row>
+    <row r="124" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="14" t="s">
         <v>147</v>
       </c>
@@ -5457,12 +5615,13 @@
       <c r="D124" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="E124" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F124" s="14"/>
-    </row>
-    <row r="125" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E124" s="14"/>
+      <c r="F124" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G124" s="14"/>
+    </row>
+    <row r="125" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="14" t="s">
         <v>370</v>
       </c>
@@ -5475,12 +5634,13 @@
       <c r="D125" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E125" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F125" s="14"/>
-    </row>
-    <row r="126" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E125" s="14"/>
+      <c r="F125" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G125" s="14"/>
+    </row>
+    <row r="126" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="14" t="s">
         <v>371</v>
       </c>
@@ -5493,12 +5653,13 @@
       <c r="D126" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E126" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F126" s="14"/>
-    </row>
-    <row r="127" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E126" s="14"/>
+      <c r="F126" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G126" s="14"/>
+    </row>
+    <row r="127" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="14" t="s">
         <v>372</v>
       </c>
@@ -5511,15 +5672,16 @@
       <c r="D127" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="E127" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F127" s="14"/>
-      <c r="G127" s="15" t="s">
+      <c r="E127" s="14"/>
+      <c r="F127" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G127" s="14"/>
+      <c r="H127" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="14" t="s">
         <v>375</v>
       </c>
@@ -5532,15 +5694,16 @@
       <c r="D128" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="E128" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F128" s="14"/>
-      <c r="G128" s="15" t="s">
+      <c r="E128" s="14"/>
+      <c r="F128" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G128" s="14"/>
+      <c r="H128" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="14" t="s">
         <v>377</v>
       </c>
@@ -5553,15 +5716,16 @@
       <c r="D129" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="E129" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F129" s="14"/>
-      <c r="G129" s="15" t="s">
+      <c r="E129" s="14"/>
+      <c r="F129" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G129" s="14"/>
+      <c r="H129" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
         <v>380</v>
       </c>
@@ -5574,15 +5738,16 @@
       <c r="D130" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="E130" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F130" s="14"/>
-      <c r="G130" s="15" t="s">
+      <c r="E130" s="14"/>
+      <c r="F130" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G130" s="14"/>
+      <c r="H130" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="14" t="s">
         <v>383</v>
       </c>
@@ -5595,15 +5760,16 @@
       <c r="D131" s="14" t="s">
         <v>384</v>
       </c>
-      <c r="E131" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F131" s="14"/>
-      <c r="G131" s="15" t="s">
+      <c r="E131" s="14"/>
+      <c r="F131" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G131" s="14"/>
+      <c r="H131" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="14" t="s">
         <v>385</v>
       </c>
@@ -5616,15 +5782,16 @@
       <c r="D132" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="E132" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F132" s="14"/>
-      <c r="G132" s="15" t="s">
+      <c r="E132" s="14"/>
+      <c r="F132" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G132" s="14"/>
+      <c r="H132" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="14" t="s">
         <v>387</v>
       </c>
@@ -5637,15 +5804,16 @@
       <c r="D133" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="E133" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F133" s="14"/>
-      <c r="G133" s="15" t="s">
+      <c r="E133" s="14"/>
+      <c r="F133" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G133" s="14"/>
+      <c r="H133" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="14" t="s">
         <v>389</v>
       </c>
@@ -5658,15 +5826,16 @@
       <c r="D134" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="E134" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F134" s="14"/>
-      <c r="G134" s="15" t="s">
+      <c r="E134" s="14"/>
+      <c r="F134" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G134" s="14"/>
+      <c r="H134" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="14" t="s">
         <v>391</v>
       </c>
@@ -5679,15 +5848,16 @@
       <c r="D135" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="E135" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F135" s="14"/>
-      <c r="G135" s="15" t="s">
+      <c r="E135" s="14"/>
+      <c r="F135" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G135" s="14"/>
+      <c r="H135" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="14" t="s">
         <v>394</v>
       </c>
@@ -5700,15 +5870,16 @@
       <c r="D136" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="E136" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F136" s="14"/>
-      <c r="G136" s="15" t="s">
+      <c r="E136" s="14"/>
+      <c r="F136" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G136" s="14"/>
+      <c r="H136" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="14" t="s">
         <v>397</v>
       </c>
@@ -5721,15 +5892,16 @@
       <c r="D137" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="E137" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F137" s="14"/>
-      <c r="G137" s="15" t="s">
+      <c r="E137" s="16"/>
+      <c r="F137" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G137" s="14"/>
+      <c r="H137" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="16" t="s">
         <v>398</v>
       </c>
@@ -5739,11 +5911,12 @@
       <c r="D138" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="G138" s="15" t="s">
+      <c r="E138" s="16"/>
+      <c r="H138" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="14" t="s">
         <v>401</v>
       </c>
@@ -5756,15 +5929,16 @@
       <c r="D139" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="E139" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F139" s="14"/>
-      <c r="G139" s="15" t="s">
+      <c r="E139" s="14"/>
+      <c r="F139" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G139" s="14"/>
+      <c r="H139" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="14" t="s">
         <v>403</v>
       </c>
@@ -5777,20 +5951,21 @@
       <c r="D140" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="E140" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F140" s="14"/>
-      <c r="G140" s="15" t="s">
+      <c r="E140" s="14"/>
+      <c r="F140" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G140" s="14"/>
+      <c r="H140" s="15" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
   </mergeCells>

</xml_diff>